<commit_message>
Refactor: Fixed naming of models (custom)
</commit_message>
<xml_diff>
--- a/results/rageval_ita_results.xlsx
+++ b/results/rageval_ita_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9120"/>
+    <workbookView windowWidth="20400" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,10 +152,10 @@
     <t>111M</t>
   </si>
   <si>
-    <t>ArchitRastogi/e5_small_v2_final_tuned__custom_fine_tuned_c4_base_isintfloat/e5-small-v2</t>
+    <t>intfloat/e5-small-v2 (finetuned)</t>
   </si>
   <si>
-    <t>ArchitRastogi/e5_multilingual_small_final_tuned__custom_fine_tuned_c4_base_isintfloat/multilingual-e5-small</t>
+    <t>intfloat/multilingual-e5-small (finetuned)</t>
   </si>
 </sst>
 </file>
@@ -1147,13 +1147,13 @@
   <sheetPr/>
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="61.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="107.555555555556" customWidth="1"/>
     <col min="2" max="2" width="4.66666666666667" customWidth="1"/>
     <col min="7" max="7" width="19.7777777777778" customWidth="1"/>
   </cols>

</xml_diff>